<commit_message>
Added "Timber" to race types.
</commit_message>
<xml_diff>
--- a/Data/races.xlsx
+++ b/Data/races.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uipathstuff\UiPath\EQAttempt1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2630CE-87BD-4B95-A709-E3A073F81003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A379054-98DC-42CE-8EDA-22457D65614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{871C8542-E977-409E-A001-2BE93B22B173}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{871C8542-E977-409E-A001-2BE93B22B173}"/>
   </bookViews>
   <sheets>
-    <sheet name="Thursday" sheetId="3" r:id="rId1"/>
-    <sheet name="Tuesday" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Friday" sheetId="4" r:id="rId1"/>
+    <sheet name="Thursday" sheetId="3" r:id="rId2"/>
+    <sheet name="Wednesday" sheetId="5" r:id="rId3"/>
+    <sheet name="Saturday" sheetId="6" r:id="rId4"/>
+    <sheet name="Tuesday" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="143">
   <si>
     <t>All Tracks</t>
   </si>
@@ -86,142 +88,376 @@
     <t>4:05 PM CT</t>
   </si>
   <si>
-    <t>4,6</t>
-  </si>
-  <si>
     <t>Fort Erie</t>
   </si>
   <si>
-    <t>4:30 PM ET</t>
-  </si>
-  <si>
-    <t>5,8</t>
-  </si>
-  <si>
     <t>Mountaineer</t>
   </si>
   <si>
     <t>7:00 PM ET</t>
   </si>
   <si>
+    <t>Assiniboia</t>
+  </si>
+  <si>
+    <t>7:30 PM CT</t>
+  </si>
+  <si>
+    <t>Saratoga</t>
+  </si>
+  <si>
+    <t>1:10 PM ET</t>
+  </si>
+  <si>
+    <t>2,3,6,9,10</t>
+  </si>
+  <si>
+    <t>Colonial Downs</t>
+  </si>
+  <si>
+    <t>11:45 AM ET</t>
+  </si>
+  <si>
+    <t>6,7,8,9,10,11,12</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>Delaware Park</t>
+  </si>
+  <si>
+    <t>12:30 PM ET</t>
+  </si>
+  <si>
+    <t>Belterra Park</t>
+  </si>
+  <si>
+    <t>12:35 PM ET</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>Del Mar</t>
+  </si>
+  <si>
+    <t>2:00 PM PT</t>
+  </si>
+  <si>
+    <t>1,4,6,8</t>
+  </si>
+  <si>
+    <t>Hawthorne</t>
+  </si>
+  <si>
+    <t>2:10 PM CT</t>
+  </si>
+  <si>
+    <t>3,7,9</t>
+  </si>
+  <si>
+    <t>4,6,8,9</t>
+  </si>
+  <si>
+    <t>Camarero</t>
+  </si>
+  <si>
+    <t>2:45 PM ET</t>
+  </si>
+  <si>
+    <t>Woodbine</t>
+  </si>
+  <si>
+    <t>4:50 PM ET</t>
+  </si>
+  <si>
+    <t>2,4,5</t>
+  </si>
+  <si>
+    <t>Canterbury Park</t>
+  </si>
+  <si>
+    <t>5:10 PM CT</t>
+  </si>
+  <si>
+    <t>2,4,6</t>
+  </si>
+  <si>
+    <t>7,8,9</t>
+  </si>
+  <si>
+    <t>Evangeline</t>
+  </si>
+  <si>
+    <t>5:30 PM CT</t>
+  </si>
+  <si>
+    <t>1,3,5,7</t>
+  </si>
+  <si>
+    <t>Penn National</t>
+  </si>
+  <si>
+    <t>5:45 PM ET</t>
+  </si>
+  <si>
+    <t>Retama Park</t>
+  </si>
+  <si>
+    <t>6:15 PM CT</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,7,9,10,11</t>
+  </si>
+  <si>
+    <t>Charles Town</t>
+  </si>
+  <si>
+    <t>Parx Racing</t>
+  </si>
+  <si>
+    <t>12:40 PM ET</t>
+  </si>
+  <si>
+    <t>4,7,9</t>
+  </si>
+  <si>
+    <t>10,11</t>
+  </si>
+  <si>
+    <t>4,7</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Arapahoe</t>
+  </si>
+  <si>
+    <t>1:00 PM MT</t>
+  </si>
+  <si>
+    <t>1:05 PM ET</t>
+  </si>
+  <si>
+    <t>1,2,5,6,8</t>
+  </si>
+  <si>
+    <t>Fair Grounds</t>
+  </si>
+  <si>
+    <t>12:00 PM CT</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Blackfoot</t>
+  </si>
+  <si>
+    <t>12:00 PM MT</t>
+  </si>
+  <si>
+    <t>1,2,3,5,7</t>
+  </si>
+  <si>
+    <t>5,7</t>
+  </si>
+  <si>
+    <t>Gulfstream Park</t>
+  </si>
+  <si>
+    <t>12:55 PM ET</t>
+  </si>
+  <si>
+    <t>1,5,9</t>
+  </si>
+  <si>
+    <t>3,5,7,9</t>
+  </si>
+  <si>
+    <t>3:00 PM PT</t>
+  </si>
+  <si>
+    <t>3:08 PM ET</t>
+  </si>
+  <si>
+    <t>2,6,7,8,9,10,11</t>
+  </si>
+  <si>
+    <t>Sweetwater Downs</t>
+  </si>
+  <si>
+    <t>4:00 PM MT</t>
+  </si>
+  <si>
+    <t>4,5,6,7</t>
+  </si>
+  <si>
+    <t>Harrah's Columbus Nebraska</t>
+  </si>
+  <si>
+    <t>4:03 PM ET</t>
+  </si>
+  <si>
+    <t>Prairie Meadows</t>
+  </si>
+  <si>
+    <t>6:00 PM CT</t>
+  </si>
+  <si>
+    <t>Lone Star</t>
+  </si>
+  <si>
+    <t>6:05 PM CT</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,7,8,9,10</t>
+  </si>
+  <si>
+    <t>Albuquerque</t>
+  </si>
+  <si>
+    <t>6:05 PM MT</t>
+  </si>
+  <si>
+    <t>5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Century Mile</t>
+  </si>
+  <si>
+    <t>6:15 PM MT</t>
+  </si>
+  <si>
     <t>1,2,3,4</t>
   </si>
   <si>
-    <t>Assiniboia</t>
-  </si>
-  <si>
-    <t>7:30 PM CT</t>
-  </si>
-  <si>
-    <t>Saratoga</t>
-  </si>
-  <si>
-    <t>1:10 PM ET</t>
-  </si>
-  <si>
-    <t>2,3,6,9,10</t>
-  </si>
-  <si>
-    <t>Colonial Downs</t>
-  </si>
-  <si>
-    <t>11:45 AM ET</t>
-  </si>
-  <si>
-    <t>6,7,8,9,10,11,12</t>
-  </si>
-  <si>
-    <t>1,2,3</t>
-  </si>
-  <si>
-    <t>Delaware Park</t>
-  </si>
-  <si>
-    <t>12:30 PM ET</t>
-  </si>
-  <si>
-    <t>Belterra Park</t>
-  </si>
-  <si>
-    <t>12:35 PM ET</t>
-  </si>
-  <si>
-    <t>1,5</t>
-  </si>
-  <si>
-    <t>Del Mar</t>
-  </si>
-  <si>
-    <t>2:00 PM PT</t>
-  </si>
-  <si>
-    <t>1,4,6,8</t>
-  </si>
-  <si>
-    <t>Hawthorne</t>
-  </si>
-  <si>
-    <t>2:10 PM CT</t>
-  </si>
-  <si>
-    <t>3,7,9</t>
-  </si>
-  <si>
-    <t>4,6,8,9</t>
-  </si>
-  <si>
-    <t>Camarero</t>
-  </si>
-  <si>
-    <t>2:45 PM ET</t>
-  </si>
-  <si>
-    <t>Woodbine</t>
-  </si>
-  <si>
-    <t>4:50 PM ET</t>
-  </si>
-  <si>
-    <t>2,4,5</t>
-  </si>
-  <si>
-    <t>Canterbury Park</t>
-  </si>
-  <si>
-    <t>5:10 PM CT</t>
-  </si>
-  <si>
-    <t>2,4,6</t>
-  </si>
-  <si>
-    <t>7,8,9</t>
-  </si>
-  <si>
-    <t>Evangeline</t>
-  </si>
-  <si>
-    <t>5:30 PM CT</t>
-  </si>
-  <si>
-    <t>1,3,5,7</t>
-  </si>
-  <si>
-    <t>Penn National</t>
-  </si>
-  <si>
-    <t>5:45 PM ET</t>
-  </si>
-  <si>
-    <t>Retama Park</t>
-  </si>
-  <si>
-    <t>6:15 PM CT</t>
-  </si>
-  <si>
-    <t>2,3,4,5,6,7,9,10,11</t>
-  </si>
-  <si>
-    <t>Charles Town</t>
+    <t>Remington Park</t>
+  </si>
+  <si>
+    <t>6:30 PM CT</t>
+  </si>
+  <si>
+    <t>1,6,9</t>
+  </si>
+  <si>
+    <t>Emerald Downs</t>
+  </si>
+  <si>
+    <t>7:00 PM PT</t>
+  </si>
+  <si>
+    <t>Hastings</t>
+  </si>
+  <si>
+    <t>11:35 AM ET</t>
+  </si>
+  <si>
+    <t>Mahoning Valley Race Course</t>
+  </si>
+  <si>
+    <t>12:15 PM ET</t>
+  </si>
+  <si>
+    <t>12:20 PM ET</t>
+  </si>
+  <si>
+    <t>1,9</t>
+  </si>
+  <si>
+    <t>Tampa Bay</t>
+  </si>
+  <si>
+    <t>5,7,9</t>
+  </si>
+  <si>
+    <t>Turf Paradise</t>
+  </si>
+  <si>
+    <t>12:40 PM MT</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>Delta Downs</t>
+  </si>
+  <si>
+    <t>4:50 PM CT</t>
+  </si>
+  <si>
+    <t>Turfway Park</t>
+  </si>
+  <si>
+    <t>5:55 PM ET</t>
+  </si>
+  <si>
+    <t>6:15 PM ET</t>
+  </si>
+  <si>
+    <t>Keeneland</t>
+  </si>
+  <si>
+    <t>3,5,8,10</t>
+  </si>
+  <si>
+    <t>Aqueduct</t>
+  </si>
+  <si>
+    <t>Fonner Park</t>
+  </si>
+  <si>
+    <t>1:30 PM CT</t>
+  </si>
+  <si>
+    <t>Monkton</t>
+  </si>
+  <si>
+    <t>1:30 PM ET</t>
+  </si>
+  <si>
+    <t>Laurel Park</t>
+  </si>
+  <si>
+    <t>12:10 PM ET</t>
+  </si>
+  <si>
+    <t>Oaklawn Park</t>
+  </si>
+  <si>
+    <t>12:20 PM CT</t>
+  </si>
+  <si>
+    <t>4,6,8,10</t>
+  </si>
+  <si>
+    <t>12:55 PM PT</t>
+  </si>
+  <si>
+    <t>3,7</t>
+  </si>
+  <si>
+    <t>Blue Ridge</t>
+  </si>
+  <si>
+    <t>2:00 PM ET</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12</t>
+  </si>
+  <si>
+    <t>Los Alamitos Quarter Horse</t>
+  </si>
+  <si>
+    <t>6:05 PM PT</t>
+  </si>
+  <si>
+    <t>4,5,6,7,8,9</t>
   </si>
 </sst>
 </file>
@@ -572,12 +808,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5AE2AB-F4B8-45E4-8A01-E92C640265FD}">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C9D9B6-D9FD-4923-9605-5392C14C4F6D}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -598,84 +840,84 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -683,16 +925,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -700,16 +942,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -717,33 +959,33 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -751,16 +993,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -768,33 +1010,33 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -802,52 +1044,120 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B15">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -857,12 +1167,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD5DD0B-6234-43A6-837E-16B87EC1DB7C}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5AE2AB-F4B8-45E4-8A01-E92C640265FD}">
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -883,16 +1201,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -900,33 +1218,33 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -934,30 +1252,30 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -968,16 +1286,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -985,16 +1303,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -1002,35 +1320,137 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1040,13 +1460,705 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA228102-1EDB-49C9-8DFF-A16A55EC7B85}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D299CB-91DD-4600-851E-351D7F28D556}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D5C474-A383-45CA-B835-C3C47D1E28F2}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD5DD0B-6234-43A6-837E-16B87EC1DB7C}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed unused variables and dependencies.
</commit_message>
<xml_diff>
--- a/Data/races.xlsx
+++ b/Data/races.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uipathstuff\UiPath\EQAttempt1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A379054-98DC-42CE-8EDA-22457D65614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E0007B-7ED7-4DF0-BBCE-5435DA74BFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{871C8542-E977-409E-A001-2BE93B22B173}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{871C8542-E977-409E-A001-2BE93B22B173}"/>
   </bookViews>
   <sheets>
     <sheet name="Friday" sheetId="4" r:id="rId1"/>
     <sheet name="Thursday" sheetId="3" r:id="rId2"/>
     <sheet name="Wednesday" sheetId="5" r:id="rId3"/>
-    <sheet name="Saturday" sheetId="6" r:id="rId4"/>
-    <sheet name="Tuesday" sheetId="2" r:id="rId5"/>
+    <sheet name="Sunday" sheetId="7" r:id="rId4"/>
+    <sheet name="Saturday" sheetId="6" r:id="rId5"/>
+    <sheet name="Tuesday" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="178">
   <si>
     <t>All Tracks</t>
   </si>
@@ -397,67 +398,172 @@
     <t>6:15 PM ET</t>
   </si>
   <si>
-    <t>Keeneland</t>
-  </si>
-  <si>
-    <t>3,5,8,10</t>
-  </si>
-  <si>
-    <t>Aqueduct</t>
-  </si>
-  <si>
-    <t>Fonner Park</t>
-  </si>
-  <si>
     <t>1:30 PM CT</t>
   </si>
   <si>
-    <t>Monkton</t>
-  </si>
-  <si>
     <t>1:30 PM ET</t>
   </si>
   <si>
-    <t>Laurel Park</t>
-  </si>
-  <si>
-    <t>12:10 PM ET</t>
-  </si>
-  <si>
-    <t>Oaklawn Park</t>
-  </si>
-  <si>
-    <t>12:20 PM CT</t>
-  </si>
-  <si>
-    <t>4,6,8,10</t>
-  </si>
-  <si>
-    <t>12:55 PM PT</t>
-  </si>
-  <si>
-    <t>3,7</t>
-  </si>
-  <si>
-    <t>Blue Ridge</t>
-  </si>
-  <si>
     <t>2:00 PM ET</t>
   </si>
   <si>
-    <t>2,3,4</t>
-  </si>
-  <si>
-    <t>1,2,3,4,5,6,7,8,9,10,11,12</t>
-  </si>
-  <si>
     <t>Los Alamitos Quarter Horse</t>
   </si>
   <si>
-    <t>6:05 PM PT</t>
-  </si>
-  <si>
-    <t>4,5,6,7,8,9</t>
+    <t>Sam Houston</t>
+  </si>
+  <si>
+    <t>1,3,4,5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Santa Anita</t>
+  </si>
+  <si>
+    <t>1:00 PM PT</t>
+  </si>
+  <si>
+    <t>Lethbridge - Rmtc</t>
+  </si>
+  <si>
+    <t>1:15 PM MT</t>
+  </si>
+  <si>
+    <t>Sunray Park</t>
+  </si>
+  <si>
+    <t>Fairmount Park</t>
+  </si>
+  <si>
+    <t>Legacy Downs</t>
+  </si>
+  <si>
+    <t>Malvern</t>
+  </si>
+  <si>
+    <t>1,3,4,5</t>
+  </si>
+  <si>
+    <t>Energy Downs 307 Horse Racing</t>
+  </si>
+  <si>
+    <t>1:30 PM MT</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6</t>
+  </si>
+  <si>
+    <t>1:35 PM CT</t>
+  </si>
+  <si>
+    <t>2,4,7,10</t>
+  </si>
+  <si>
+    <t>1:50 PM PT</t>
+  </si>
+  <si>
+    <t>Pimlico</t>
+  </si>
+  <si>
+    <t>10:30 AM ET</t>
+  </si>
+  <si>
+    <t>2,5,7,9,11,12</t>
+  </si>
+  <si>
+    <t>12:02 PM CT</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11</t>
+  </si>
+  <si>
+    <t>Miles City</t>
+  </si>
+  <si>
+    <t>12:30 AM MT</t>
+  </si>
+  <si>
+    <t>1,2,6,8</t>
+  </si>
+  <si>
+    <t>Belmont At The Big A</t>
+  </si>
+  <si>
+    <t>5,7,8,10,11</t>
+  </si>
+  <si>
+    <t>1,4,7,9,11</t>
+  </si>
+  <si>
+    <t>Monmouth Park</t>
+  </si>
+  <si>
+    <t>4,6,8</t>
+  </si>
+  <si>
+    <t>2:30 PM PT</t>
+  </si>
+  <si>
+    <t>3:10 PM ET</t>
+  </si>
+  <si>
+    <t>3:45 PM MT</t>
+  </si>
+  <si>
+    <t>2,4,8</t>
+  </si>
+  <si>
+    <t>Churchill Downs</t>
+  </si>
+  <si>
+    <t>6:00 PM ET</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,8,9</t>
+  </si>
+  <si>
+    <t>6:50 PM PT</t>
+  </si>
+  <si>
+    <t>1,4,6,8,10</t>
+  </si>
+  <si>
+    <t>5,6,8,9</t>
+  </si>
+  <si>
+    <t>2,3,4,5</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>2,5,8</t>
+  </si>
+  <si>
+    <t>12:30 PM MT</t>
+  </si>
+  <si>
+    <t>1,4,6</t>
+  </si>
+  <si>
+    <t>12:45 PM ET</t>
+  </si>
+  <si>
+    <t>2,6,9</t>
+  </si>
+  <si>
+    <t>1,4,8</t>
+  </si>
+  <si>
+    <t>2:40 PM CT</t>
+  </si>
+  <si>
+    <t>4:00 PM CT</t>
+  </si>
+  <si>
+    <t>6:10 PM PT</t>
+  </si>
+  <si>
+    <t>8,9</t>
   </si>
 </sst>
 </file>
@@ -1650,10 +1756,386 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D5C474-A383-45CA-B835-C3C47D1E28F2}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B2DB928-4585-4590-BE78-309BA49E849E}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>176</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00D5C474-A383-45CA-B835-C3C47D1E28F2}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1682,33 +2164,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1716,13 +2198,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1733,13 +2215,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1750,13 +2232,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1767,13 +2249,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1784,13 +2266,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1801,84 +2283,84 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
+        <v>141</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -1886,69 +2368,341 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
+        <v>146</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B16">
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>160</v>
+      </c>
+      <c r="B29">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31">
+        <v>7</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>60</v>
       </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1957,7 +2711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD5DD0B-6234-43A6-837E-16B87EC1DB7C}">
   <dimension ref="A1:E11"/>
   <sheetViews>

</xml_diff>